<commit_message>
Added feature test script for MAR-21
</commit_message>
<xml_diff>
--- a/My Stuff/Useful git.xlsx
+++ b/My Stuff/Useful git.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\MarTech\My Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\MarTech\My Stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632D243C-E79F-4062-9B90-72D9C3D411EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039E8E42-E0D7-4663-952A-1087E2B23FE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1738D085-A1E9-4F43-A70F-7BC6327270A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Description</t>
   </si>
@@ -55,6 +55,13 @@
   </si>
   <si>
     <t>git reset --hard head</t>
+  </si>
+  <si>
+    <t>Checkout remote branch</t>
+  </si>
+  <si>
+    <t>git fetch
+git checkout [name of remote branch]</t>
   </si>
 </sst>
 </file>
@@ -90,8 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807C26D6-02FF-46B3-B825-557ADF6E0CF6}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +468,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>